<commit_message>
add meeting details 10.2
</commit_message>
<xml_diff>
--- a/final_project/else/기능명세서 통합.xlsx
+++ b/final_project/else/기능명세서 통합.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goott2\Documents\카카오톡 받은 파일\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jingo\OneDrive\바탕 화면\새 폴더\goott_lecture\final_project\else\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA41E381-B2E9-4BCA-B760-32E7C09D92E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FBDA52-350F-4919-A510-CD116F82B8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F4C56D4A-47A3-40B6-9AB2-20F18E3FB939}"/>
+    <workbookView xWindow="3075" yWindow="1110" windowWidth="13260" windowHeight="12600" xr2:uid="{F4C56D4A-47A3-40B6-9AB2-20F18E3FB939}"/>
   </bookViews>
   <sheets>
     <sheet name="통합" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="768">
   <si>
     <t>회원 가입</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2872,7 +2872,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2895,18 +2895,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6F8F9"/>
-        <bgColor rgb="FFF6F8F9"/>
       </patternFill>
     </fill>
   </fills>
@@ -3392,7 +3380,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3544,6 +3532,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3592,10 +3583,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3604,37 +3613,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4003,8 +3985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F191F85-2262-49C0-9469-D61EEDDEFCEB}">
   <dimension ref="B1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="F22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4025,42 +4007,42 @@
   <sheetData>
     <row r="1" spans="2:15" ht="14.25" thickBot="1"/>
     <row r="2" spans="2:15" ht="16.5" customHeight="1">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>313</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="57"/>
     </row>
     <row r="3" spans="2:15" ht="16.5" customHeight="1">
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="57"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="59"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="60"/>
     </row>
     <row r="5" spans="2:15" ht="14.25" thickBot="1">
-      <c r="B5" s="60"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="62"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="63"/>
     </row>
     <row r="6" spans="2:15" ht="25.5" customHeight="1" thickBot="1">
       <c r="B6" s="37" t="s">
@@ -4069,13 +4051,13 @@
       <c r="C6" s="37" t="s">
         <v>712</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="64" t="s">
         <v>353</v>
       </c>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="66"/>
       <c r="J6" s="36" t="s">
         <v>713</v>
       </c>
@@ -4090,7 +4072,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" ht="25.5" customHeight="1">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>664</v>
       </c>
       <c r="C7" s="38" t="s">
@@ -4115,7 +4097,7 @@
       <c r="K7" s="36" t="s">
         <v>665</v>
       </c>
-      <c r="L7" s="81" t="s">
+      <c r="L7" s="51" t="s">
         <v>759</v>
       </c>
       <c r="N7" s="36" t="s">
@@ -4126,7 +4108,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" ht="25.5" customHeight="1">
-      <c r="B8" s="52"/>
+      <c r="B8" s="53"/>
       <c r="C8" s="39" t="s">
         <v>55</v>
       </c>
@@ -4146,7 +4128,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" ht="25.5" customHeight="1">
-      <c r="B9" s="52"/>
+      <c r="B9" s="53"/>
       <c r="C9" s="39" t="s">
         <v>58</v>
       </c>
@@ -4171,12 +4153,12 @@
       <c r="K9" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="L9" s="81" t="s">
+      <c r="L9" s="51" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="25.5" customHeight="1">
-      <c r="B10" s="52"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="39" t="s">
         <v>672</v>
       </c>
@@ -4190,7 +4172,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" ht="25.5" customHeight="1">
-      <c r="B11" s="52"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="39" t="s">
         <v>673</v>
       </c>
@@ -4204,7 +4186,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B12" s="53"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="40" t="s">
         <v>674</v>
       </c>
@@ -4213,12 +4195,12 @@
       <c r="F12" s="49"/>
       <c r="G12" s="49"/>
       <c r="H12" s="50"/>
-      <c r="L12" s="81" t="s">
+      <c r="L12" s="51" t="s">
         <v>725</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="25.5" customHeight="1">
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="52" t="s">
         <v>216</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4232,7 +4214,7 @@
       <c r="K13" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="L13" s="81" t="s">
+      <c r="L13" s="51" t="s">
         <v>284</v>
       </c>
       <c r="M13" s="36" t="s">
@@ -4240,7 +4222,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" ht="25.5" customHeight="1">
-      <c r="B14" s="52"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="39" t="s">
         <v>678</v>
       </c>
@@ -4249,7 +4231,7 @@
       <c r="F14" s="46"/>
       <c r="G14" s="46"/>
       <c r="H14" s="47"/>
-      <c r="L14" s="81" t="s">
+      <c r="L14" s="51" t="s">
         <v>282</v>
       </c>
       <c r="M14" s="36" t="s">
@@ -4257,7 +4239,7 @@
       </c>
     </row>
     <row r="15" spans="2:15" ht="25.5" customHeight="1">
-      <c r="B15" s="52"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="39" t="s">
         <v>40</v>
       </c>
@@ -4277,12 +4259,12 @@
       <c r="K15" s="36" t="s">
         <v>723</v>
       </c>
-      <c r="L15" s="81" t="s">
+      <c r="L15" s="51" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B16" s="53"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="41" t="s">
         <v>38</v>
       </c>
@@ -4295,12 +4277,12 @@
       <c r="F16" s="49"/>
       <c r="G16" s="49"/>
       <c r="H16" s="50"/>
-      <c r="L16" s="81" t="s">
+      <c r="L16" s="51" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="52" t="s">
         <v>683</v>
       </c>
       <c r="C17" s="38" t="s">
@@ -4319,7 +4301,7 @@
       </c>
     </row>
     <row r="18" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B18" s="52"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="39" t="s">
         <v>684</v>
       </c>
@@ -4339,10 +4321,10 @@
       <c r="K18" s="36" t="s">
         <v>673</v>
       </c>
-      <c r="L18" s="81"/>
+      <c r="L18" s="51"/>
     </row>
     <row r="19" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B19" s="52"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="39" t="s">
         <v>688</v>
       </c>
@@ -4354,10 +4336,10 @@
       <c r="K19" s="36" t="s">
         <v>726</v>
       </c>
-      <c r="L19" s="81"/>
+      <c r="L19" s="51"/>
     </row>
     <row r="20" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B20" s="52"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="39" t="s">
         <v>689</v>
       </c>
@@ -4377,7 +4359,7 @@
       </c>
     </row>
     <row r="21" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B21" s="52"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="39" t="s">
         <v>690</v>
       </c>
@@ -4394,7 +4376,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B22" s="53"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="41" t="s">
         <v>691</v>
       </c>
@@ -4411,7 +4393,7 @@
       </c>
     </row>
     <row r="23" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="52" t="s">
         <v>709</v>
       </c>
       <c r="C23" s="38" t="s">
@@ -4436,7 +4418,7 @@
       </c>
     </row>
     <row r="24" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B24" s="52"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="39" t="s">
         <v>694</v>
       </c>
@@ -4453,7 +4435,7 @@
       </c>
     </row>
     <row r="25" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B25" s="52"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="39" t="s">
         <v>695</v>
       </c>
@@ -4467,7 +4449,7 @@
       </c>
     </row>
     <row r="26" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B26" s="52"/>
+      <c r="B26" s="53"/>
       <c r="C26" s="39" t="s">
         <v>696</v>
       </c>
@@ -4482,7 +4464,7 @@
       <c r="H26" s="47"/>
     </row>
     <row r="27" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B27" s="52"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="39" t="s">
         <v>697</v>
       </c>
@@ -4509,7 +4491,7 @@
       </c>
     </row>
     <row r="28" spans="2:14" ht="24" customHeight="1" thickBot="1">
-      <c r="B28" s="53"/>
+      <c r="B28" s="54"/>
       <c r="C28" s="41" t="s">
         <v>698</v>
       </c>
@@ -4547,9 +4529,6 @@
       </c>
     </row>
     <row r="31" spans="2:14" ht="26.25" customHeight="1">
-      <c r="C31" s="79" t="s">
-        <v>104</v>
-      </c>
       <c r="J31" s="36" t="s">
         <v>765</v>
       </c>
@@ -4558,9 +4537,6 @@
       </c>
     </row>
     <row r="32" spans="2:14" ht="26.25" customHeight="1">
-      <c r="C32" s="80" t="s">
-        <v>114</v>
-      </c>
       <c r="J32" s="36" t="s">
         <v>766</v>
       </c>
@@ -4568,10 +4544,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="33" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C33" s="79" t="s">
-        <v>94</v>
-      </c>
+    <row r="33" spans="10:12" ht="26.25" customHeight="1">
       <c r="K33" s="36" t="s">
         <v>738</v>
       </c>
@@ -4579,34 +4552,22 @@
         <v>686</v>
       </c>
     </row>
-    <row r="34" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C34" s="80" t="s">
-        <v>112</v>
-      </c>
+    <row r="34" spans="10:12" ht="26.25" customHeight="1">
       <c r="L34" s="36" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="35" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C35" s="79" t="s">
-        <v>89</v>
-      </c>
+    <row r="35" spans="10:12" ht="26.25" customHeight="1">
       <c r="L35" s="36" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C36" s="80" t="s">
-        <v>109</v>
-      </c>
+    <row r="36" spans="10:12" ht="26.25" customHeight="1">
       <c r="L36" s="36" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="37" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C37" s="79" t="s">
-        <v>106</v>
-      </c>
+    <row r="37" spans="10:12" ht="26.25" customHeight="1">
       <c r="K37" s="36" t="s">
         <v>740</v>
       </c>
@@ -4614,26 +4575,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C38" s="80" t="s">
-        <v>105</v>
-      </c>
+    <row r="38" spans="10:12" ht="26.25" customHeight="1">
       <c r="L38" s="36" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="39" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C39" s="79" t="s">
-        <v>103</v>
-      </c>
+    <row r="39" spans="10:12" ht="26.25" customHeight="1">
       <c r="L39" s="36" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="40" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C40" s="80" t="s">
-        <v>102</v>
-      </c>
+    <row r="40" spans="10:12" ht="26.25" customHeight="1">
       <c r="J40" s="36" t="s">
         <v>709</v>
       </c>
@@ -4644,10 +4596,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="41" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C41" s="79" t="s">
-        <v>87</v>
-      </c>
+    <row r="41" spans="10:12" ht="26.25" customHeight="1">
       <c r="J41" s="36" t="s">
         <v>764</v>
       </c>
@@ -4655,10 +4604,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="42" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C42" s="80" t="s">
-        <v>100</v>
-      </c>
+    <row r="42" spans="10:12" ht="26.25" customHeight="1">
       <c r="J42" s="36" t="s">
         <v>767</v>
       </c>
@@ -4666,10 +4612,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="43" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C43" s="79" t="s">
-        <v>98</v>
-      </c>
+    <row r="43" spans="10:12" ht="26.25" customHeight="1">
       <c r="K43" s="36" t="s">
         <v>317</v>
       </c>
@@ -4677,26 +4620,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C44" s="80" t="s">
-        <v>97</v>
-      </c>
+    <row r="44" spans="10:12" ht="26.25" customHeight="1">
       <c r="L44" s="36" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C45" s="79" t="s">
-        <v>96</v>
-      </c>
+    <row r="45" spans="10:12" ht="26.25" customHeight="1">
       <c r="L45" s="36" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C46" s="80" t="s">
-        <v>95</v>
-      </c>
+    <row r="46" spans="10:12" ht="26.25" customHeight="1">
       <c r="K46" s="36" t="s">
         <v>746</v>
       </c>
@@ -4704,57 +4638,45 @@
         <v>374</v>
       </c>
     </row>
-    <row r="47" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C47" s="79" t="s">
-        <v>93</v>
-      </c>
+    <row r="47" spans="10:12" ht="26.25" customHeight="1">
       <c r="L47" s="36" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="48" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C48" s="80" t="s">
-        <v>92</v>
-      </c>
+    <row r="48" spans="10:12" ht="26.25" customHeight="1">
       <c r="L48" s="36" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="49" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C49" s="79" t="s">
-        <v>91</v>
-      </c>
+    <row r="49" spans="11:12" ht="26.25" customHeight="1">
       <c r="L49" s="36" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="50" spans="3:12" ht="26.25" customHeight="1">
-      <c r="C50" s="80" t="s">
-        <v>90</v>
-      </c>
+    <row r="50" spans="11:12" ht="26.25" customHeight="1">
       <c r="L50" s="36" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="51" spans="3:12" ht="26.25" customHeight="1">
+    <row r="51" spans="11:12" ht="26.25" customHeight="1">
       <c r="K51" s="36" t="s">
         <v>749</v>
       </c>
       <c r="L51" s="36" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="52" spans="3:12" ht="26.25" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="11:12" ht="26.25" customHeight="1">
       <c r="L52" s="36" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="3:12" ht="26.25" customHeight="1">
+    <row r="53" spans="11:12" ht="26.25" customHeight="1">
       <c r="L53" s="36" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="3:12" ht="23.25" customHeight="1">
+    <row r="54" spans="11:12" ht="23.25" customHeight="1">
       <c r="K54" s="36" t="s">
         <v>750</v>
       </c>
@@ -4762,17 +4684,17 @@
         <v>751</v>
       </c>
     </row>
-    <row r="55" spans="3:12" ht="28.5" customHeight="1">
+    <row r="55" spans="11:12" ht="28.5" customHeight="1">
       <c r="L55" s="36" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="56" spans="3:12" ht="28.5" customHeight="1">
+    <row r="56" spans="11:12" ht="28.5" customHeight="1">
       <c r="L56" s="36" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="57" spans="3:12" ht="28.5" customHeight="1">
+    <row r="57" spans="11:12" ht="28.5" customHeight="1">
       <c r="K57" s="36" t="s">
         <v>754</v>
       </c>
@@ -4780,17 +4702,17 @@
         <v>755</v>
       </c>
     </row>
-    <row r="58" spans="3:12" ht="28.5" customHeight="1">
+    <row r="58" spans="11:12" ht="28.5" customHeight="1">
       <c r="L58" s="36" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="59" spans="3:12" ht="28.5" customHeight="1"/>
-    <row r="60" spans="3:12" ht="28.5" customHeight="1"/>
-    <row r="61" spans="3:12" ht="28.5" customHeight="1"/>
-    <row r="62" spans="3:12" ht="28.5" customHeight="1"/>
-    <row r="63" spans="3:12" ht="28.5" customHeight="1"/>
-    <row r="64" spans="3:12" ht="28.5" customHeight="1"/>
+    <row r="59" spans="11:12" ht="28.5" customHeight="1"/>
+    <row r="60" spans="11:12" ht="28.5" customHeight="1"/>
+    <row r="61" spans="11:12" ht="28.5" customHeight="1"/>
+    <row r="62" spans="11:12" ht="28.5" customHeight="1"/>
+    <row r="63" spans="11:12" ht="28.5" customHeight="1"/>
+    <row r="64" spans="11:12" ht="28.5" customHeight="1"/>
     <row r="65" ht="28.5" customHeight="1"/>
     <row r="66" ht="28.5" customHeight="1"/>
     <row r="67" ht="28.5" customHeight="1"/>
@@ -4806,9 +4728,6 @@
     <mergeCell ref="D6:H6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="C31:C50" xr:uid="{BCFCC327-D2C7-4BF8-A6DC-A1590D2F6937}"/>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5939,11 +5858,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="67" t="s">
         <v>313</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="25" t="s">
@@ -6838,35 +6757,35 @@
   <sheetData>
     <row r="4" spans="3:17" ht="17.25" thickBot="1"/>
     <row r="5" spans="3:17">
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77" t="s">
+      <c r="D5" s="72"/>
+      <c r="E5" s="72" t="s">
         <v>354</v>
       </c>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77" t="s">
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72" t="s">
         <v>353</v>
       </c>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77" t="s">
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="78"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="73"/>
     </row>
     <row r="6" spans="3:17">
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="70" t="s">
         <v>312</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="68" t="s">
         <v>352</v>
       </c>
@@ -6883,14 +6802,14 @@
       <c r="N6" s="68"/>
       <c r="O6" s="68"/>
       <c r="P6" s="68"/>
-      <c r="Q6" s="75"/>
+      <c r="Q6" s="69"/>
     </row>
     <row r="7" spans="3:17">
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="70" t="s">
         <v>288</v>
       </c>
-      <c r="D7" s="72"/>
-      <c r="E7" s="67" t="s">
+      <c r="D7" s="71"/>
+      <c r="E7" s="75" t="s">
         <v>350</v>
       </c>
       <c r="F7" s="68"/>
@@ -6906,12 +6825,12 @@
       <c r="N7" s="68"/>
       <c r="O7" s="68"/>
       <c r="P7" s="68"/>
-      <c r="Q7" s="75"/>
+      <c r="Q7" s="69"/>
     </row>
     <row r="8" spans="3:17">
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="67" t="s">
+      <c r="C8" s="70"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="75" t="s">
         <v>348</v>
       </c>
       <c r="F8" s="68"/>
@@ -6927,14 +6846,14 @@
       <c r="N8" s="68"/>
       <c r="O8" s="68"/>
       <c r="P8" s="68"/>
-      <c r="Q8" s="75"/>
+      <c r="Q8" s="69"/>
     </row>
     <row r="9" spans="3:17">
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="70" t="s">
         <v>275</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="67" t="s">
+      <c r="D9" s="71"/>
+      <c r="E9" s="75" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="68"/>
@@ -6950,12 +6869,12 @@
       <c r="N9" s="68"/>
       <c r="O9" s="68"/>
       <c r="P9" s="68"/>
-      <c r="Q9" s="75"/>
+      <c r="Q9" s="69"/>
     </row>
     <row r="10" spans="3:17">
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="67" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="75" t="s">
         <v>345</v>
       </c>
       <c r="F10" s="68"/>
@@ -6973,12 +6892,12 @@
       </c>
       <c r="O10" s="68"/>
       <c r="P10" s="68"/>
-      <c r="Q10" s="75"/>
+      <c r="Q10" s="69"/>
     </row>
     <row r="11" spans="3:17">
-      <c r="C11" s="71"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="67" t="s">
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="75" t="s">
         <v>342</v>
       </c>
       <c r="F11" s="68"/>
@@ -6994,13 +6913,13 @@
       <c r="N11" s="68"/>
       <c r="O11" s="68"/>
       <c r="P11" s="68"/>
-      <c r="Q11" s="75"/>
+      <c r="Q11" s="69"/>
     </row>
     <row r="12" spans="3:17">
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="70" t="s">
         <v>218</v>
       </c>
-      <c r="D12" s="72"/>
+      <c r="D12" s="71"/>
       <c r="E12" s="68" t="s">
         <v>340</v>
       </c>
@@ -7017,11 +6936,11 @@
       <c r="N12" s="68"/>
       <c r="O12" s="68"/>
       <c r="P12" s="68"/>
-      <c r="Q12" s="75"/>
+      <c r="Q12" s="69"/>
     </row>
     <row r="13" spans="3:17">
-      <c r="C13" s="71"/>
-      <c r="D13" s="72"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="68" t="s">
         <v>338</v>
       </c>
@@ -7038,13 +6957,13 @@
       <c r="N13" s="68"/>
       <c r="O13" s="68"/>
       <c r="P13" s="68"/>
-      <c r="Q13" s="75"/>
+      <c r="Q13" s="69"/>
     </row>
     <row r="14" spans="3:17">
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="70" t="s">
         <v>198</v>
       </c>
-      <c r="D14" s="72"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="68" t="s">
         <v>336</v>
       </c>
@@ -7061,11 +6980,11 @@
       <c r="N14" s="68"/>
       <c r="O14" s="68"/>
       <c r="P14" s="68"/>
-      <c r="Q14" s="75"/>
+      <c r="Q14" s="69"/>
     </row>
     <row r="15" spans="3:17">
-      <c r="C15" s="71"/>
-      <c r="D15" s="72"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="71"/>
       <c r="E15" s="68" t="s">
         <v>334</v>
       </c>
@@ -7082,13 +7001,13 @@
       <c r="N15" s="68"/>
       <c r="O15" s="68"/>
       <c r="P15" s="68"/>
-      <c r="Q15" s="75"/>
+      <c r="Q15" s="69"/>
     </row>
     <row r="16" spans="3:17">
-      <c r="C16" s="71" t="s">
+      <c r="C16" s="70" t="s">
         <v>332</v>
       </c>
-      <c r="D16" s="72"/>
+      <c r="D16" s="71"/>
       <c r="E16" s="68" t="s">
         <v>331</v>
       </c>
@@ -7105,11 +7024,11 @@
       <c r="N16" s="68"/>
       <c r="O16" s="68"/>
       <c r="P16" s="68"/>
-      <c r="Q16" s="75"/>
+      <c r="Q16" s="69"/>
     </row>
     <row r="17" spans="3:17">
-      <c r="C17" s="71"/>
-      <c r="D17" s="72"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="71"/>
       <c r="E17" s="68" t="s">
         <v>276</v>
       </c>
@@ -7126,11 +7045,11 @@
       <c r="N17" s="68"/>
       <c r="O17" s="68"/>
       <c r="P17" s="68"/>
-      <c r="Q17" s="75"/>
+      <c r="Q17" s="69"/>
     </row>
     <row r="18" spans="3:17">
-      <c r="C18" s="71"/>
-      <c r="D18" s="72"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="68" t="s">
         <v>317</v>
       </c>
@@ -7147,11 +7066,11 @@
       <c r="N18" s="68"/>
       <c r="O18" s="68"/>
       <c r="P18" s="68"/>
-      <c r="Q18" s="75"/>
+      <c r="Q18" s="69"/>
     </row>
     <row r="19" spans="3:17">
-      <c r="C19" s="71"/>
-      <c r="D19" s="72"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="68" t="s">
         <v>327</v>
       </c>
@@ -7168,13 +7087,13 @@
       <c r="N19" s="68"/>
       <c r="O19" s="68"/>
       <c r="P19" s="68"/>
-      <c r="Q19" s="75"/>
+      <c r="Q19" s="69"/>
     </row>
     <row r="20" spans="3:17">
-      <c r="C20" s="71" t="s">
+      <c r="C20" s="70" t="s">
         <v>325</v>
       </c>
-      <c r="D20" s="72"/>
+      <c r="D20" s="71"/>
       <c r="E20" s="68" t="s">
         <v>41</v>
       </c>
@@ -7191,11 +7110,11 @@
       <c r="N20" s="68"/>
       <c r="O20" s="68"/>
       <c r="P20" s="68"/>
-      <c r="Q20" s="75"/>
+      <c r="Q20" s="69"/>
     </row>
     <row r="21" spans="3:17">
-      <c r="C21" s="71"/>
-      <c r="D21" s="72"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="71"/>
       <c r="E21" s="68" t="s">
         <v>145</v>
       </c>
@@ -7212,11 +7131,11 @@
       <c r="N21" s="68"/>
       <c r="O21" s="68"/>
       <c r="P21" s="68"/>
-      <c r="Q21" s="75"/>
+      <c r="Q21" s="69"/>
     </row>
     <row r="22" spans="3:17">
-      <c r="C22" s="71"/>
-      <c r="D22" s="72"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="71"/>
       <c r="E22" s="68" t="s">
         <v>322</v>
       </c>
@@ -7235,11 +7154,11 @@
       </c>
       <c r="O22" s="68"/>
       <c r="P22" s="68"/>
-      <c r="Q22" s="75"/>
+      <c r="Q22" s="69"/>
     </row>
     <row r="23" spans="3:17">
-      <c r="C23" s="71"/>
-      <c r="D23" s="72"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="71"/>
       <c r="E23" s="68" t="s">
         <v>319</v>
       </c>
@@ -7256,11 +7175,11 @@
       <c r="N23" s="68"/>
       <c r="O23" s="68"/>
       <c r="P23" s="68"/>
-      <c r="Q23" s="75"/>
+      <c r="Q23" s="69"/>
     </row>
     <row r="24" spans="3:17">
-      <c r="C24" s="71"/>
-      <c r="D24" s="72"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="71"/>
       <c r="E24" s="68" t="s">
         <v>317</v>
       </c>
@@ -7277,37 +7196,80 @@
       <c r="N24" s="68"/>
       <c r="O24" s="68"/>
       <c r="P24" s="68"/>
-      <c r="Q24" s="75"/>
+      <c r="Q24" s="69"/>
     </row>
     <row r="25" spans="3:17" ht="17.25" thickBot="1">
-      <c r="C25" s="73"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="69" t="s">
+      <c r="C25" s="78"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="76" t="s">
         <v>315</v>
       </c>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69" t="s">
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76" t="s">
         <v>314</v>
       </c>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="69"/>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="69"/>
-      <c r="Q25" s="70"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="76"/>
+      <c r="N25" s="76"/>
+      <c r="O25" s="76"/>
+      <c r="P25" s="76"/>
+      <c r="Q25" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="N23:Q23"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="C20:D25"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="C9:D11"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="C16:D19"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:M14"/>
     <mergeCell ref="C12:D13"/>
     <mergeCell ref="N21:Q21"/>
     <mergeCell ref="N20:Q20"/>
@@ -7324,55 +7286,12 @@
     <mergeCell ref="N16:Q16"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="H16:M16"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:M14"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="H7:M7"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="C20:D25"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="C9:D11"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="C16:D19"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="N23:Q23"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H23:M23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10175,5 +10094,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>